<commit_message>
feat(excel2json-lists): enable to add comments to list nodes (RDU-18) (#1111)
</commit_message>
<xml_diff>
--- a/docs/assets/data_model_templates/lists/new_lists.xlsx
+++ b/docs/assets/data_model_templates/lists/new_lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/docs/assets/data_model_templates/lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CA5934-B8AC-5242-B691-E9B30FCB8EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3561C370-397B-3344-8C72-6DF20F749B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28860" windowHeight="20480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29800" yWindow="4560" windowWidth="29320" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="list 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="60">
   <si>
     <t>ID (optional)</t>
   </si>
@@ -179,17 +179,51 @@
   </si>
   <si>
     <t>rm_2</t>
+  </si>
+  <si>
+    <t>en_comments</t>
+  </si>
+  <si>
+    <t>de_comments</t>
+  </si>
+  <si>
+    <t>fr_comments</t>
+  </si>
+  <si>
+    <t>it_comments</t>
+  </si>
+  <si>
+    <t>rm_comments</t>
+  </si>
+  <si>
+    <t>Comment for the list.</t>
+  </si>
+  <si>
+    <t>Kommentar für die Liste</t>
+  </si>
+  <si>
+    <t>Comment for the third node.</t>
+  </si>
+  <si>
+    <t>Kommentar für den dritten Knoten.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -248,11 +282,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -469,351 +504,379 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView zoomScale="142" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
-    <col min="10" max="26" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" customWidth="1"/>
+    <col min="12" max="28" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="4"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1802,7 +1865,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="A1">
     <cfRule type="colorScale" priority="1">
       <colorScale>
@@ -1820,65 +1883,95 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783195D9-9670-BB46-AB57-45AFEA14AAC6}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView zoomScale="166" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="7" customWidth="1"/>
+    <col min="2" max="3" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" customWidth="1"/>
+    <col min="12" max="13" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1894,5 +1987,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>